<commit_message>
Assets for new classes & documentation
</commit_message>
<xml_diff>
--- a/Documents/Character List by Class.xlsx
+++ b/Documents/Character List by Class.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugob\BindingStories\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A20C49-A8AF-4DF6-9117-3FDFF4A4D3CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED630667-72CB-47E2-93FB-B89AC09E3A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -429,9 +429,6 @@
     <t>Alievra</t>
   </si>
   <si>
-    <t>Spellblade/Sageblade</t>
-  </si>
-  <si>
     <t>Celsus</t>
   </si>
   <si>
@@ -556,6 +553,9 @@
   </si>
   <si>
     <t>Pr</t>
+  </si>
+  <si>
+    <t>Spellsword/Sageblade</t>
   </si>
 </sst>
 </file>
@@ -878,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="D152" sqref="D152"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -925,7 +925,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>44</v>
@@ -1028,7 +1028,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>44</v>
@@ -1114,7 +1114,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>44</v>
@@ -1247,7 +1247,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>51</v>
@@ -1258,7 +1258,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>51</v>
@@ -1310,7 +1310,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B48" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>44</v>
@@ -1354,7 +1354,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B52" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>44</v>
@@ -1401,7 +1401,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B57" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>6</v>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B60" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>44</v>
@@ -1445,7 +1445,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B61" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>6</v>
@@ -1625,7 +1625,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B81" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>44</v>
@@ -1658,7 +1658,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B84" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>44</v>
@@ -1669,7 +1669,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B85" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>44</v>
@@ -1694,7 +1694,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B88" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>44</v>
@@ -1705,10 +1705,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>44</v>
@@ -1733,7 +1733,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B93" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>51</v>
@@ -1744,7 +1744,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B94" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>51</v>
@@ -1755,7 +1755,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B95" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>51</v>
@@ -1780,7 +1780,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B98" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>51</v>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B99" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>51</v>
@@ -1816,7 +1816,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B102" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>51</v>
@@ -1827,7 +1827,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B103" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>51</v>
@@ -1860,7 +1860,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B106" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>51</v>
@@ -1871,7 +1871,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B107" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>51</v>
@@ -1882,7 +1882,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B108" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>51</v>
@@ -1993,7 +1993,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>101</v>
@@ -2043,7 +2043,7 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B127" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>44</v>
@@ -2115,7 +2115,7 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B135" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>44</v>
@@ -2151,7 +2151,7 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B139" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>6</v>
@@ -2176,7 +2176,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B142" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>6</v>
@@ -2187,7 +2187,7 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B143" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>44</v>
@@ -2223,7 +2223,7 @@
         <v>6</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>121</v>
@@ -2240,7 +2240,7 @@
         <v>6</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>122</v>
@@ -2293,10 +2293,10 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B152" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>44</v>
@@ -2305,15 +2305,15 @@
         <v>12</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B153" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>44</v>
@@ -2322,27 +2322,27 @@
         <v>1</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B157" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B158" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B159" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>